<commit_message>
SD-added a link to add template
</commit_message>
<xml_diff>
--- a/WebContent/template/ModuleExcel.xlsx
+++ b/WebContent/template/ModuleExcel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>ModuleName</t>
   </si>
@@ -90,19 +90,55 @@
     <t>vdfv</t>
   </si>
   <si>
-    <t>fdsf</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>dadadwd</t>
-  </si>
-  <si>
-    <t>wadwd_01</t>
-  </si>
-  <si>
-    <t>wafb_01</t>
+    <t>y</t>
+  </si>
+  <si>
+    <t>works for aristos</t>
+  </si>
+  <si>
+    <t>eProject1</t>
+  </si>
+  <si>
+    <t>m-1001</t>
+  </si>
+  <si>
+    <t>m-1002</t>
+  </si>
+  <si>
+    <t>m-1003</t>
+  </si>
+  <si>
+    <t>m-1004</t>
+  </si>
+  <si>
+    <t>m-1005</t>
+  </si>
+  <si>
+    <t>p-00123</t>
+  </si>
+  <si>
+    <t>p-00124</t>
+  </si>
+  <si>
+    <t>p-00125</t>
+  </si>
+  <si>
+    <t>p-00126</t>
+  </si>
+  <si>
+    <t>p-00127</t>
+  </si>
+  <si>
+    <t>eProject2</t>
+  </si>
+  <si>
+    <t>eProject3</t>
+  </si>
+  <si>
+    <t>eProject4</t>
+  </si>
+  <si>
+    <t>eProject5</t>
   </si>
 </sst>
 </file>
@@ -121,11 +157,13 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -191,7 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -202,6 +240,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -623,57 +664,127 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>25</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>